<commit_message>
Need to fix the navigation bar
</commit_message>
<xml_diff>
--- a/iOS app (excel formula).xlsx
+++ b/iOS app (excel formula).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="23913"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="0" windowWidth="25040" windowHeight="14540" activeTab="5"/>
+    <workbookView xWindow="-320" yWindow="1200" windowWidth="25040" windowHeight="14540" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RRSP (ded'n)" sheetId="1" r:id="rId1"/>
@@ -921,7 +921,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -992,6 +992,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1266,7 +1267,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3460,8 +3461,8 @@
   </sheetPr>
   <dimension ref="A1:AD186"/>
   <sheetViews>
-    <sheetView topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="D178" sqref="D178"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3505,7 +3506,7 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="C9">
+      <c r="C9" s="18">
         <f>MIN(C6,C8)</f>
         <v>15255</v>
       </c>
@@ -3517,7 +3518,7 @@
       <c r="B11" s="8">
         <v>0.15</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="58">
         <f>$C$9*$B$11</f>
         <v>2288.25</v>
       </c>
@@ -3817,7 +3818,7 @@
         <v>54</v>
       </c>
       <c r="C66" s="22">
-        <v>40000</v>
+        <v>200000</v>
       </c>
       <c r="D66" t="s">
         <v>55</v>
@@ -3837,7 +3838,7 @@
       </c>
       <c r="C69" s="18">
         <f>$C$66*B69</f>
-        <v>1200</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -3857,9 +3858,9 @@
         <v>58</v>
       </c>
       <c r="B71" s="8"/>
-      <c r="C71">
+      <c r="C71" s="18">
         <f>MIN(C69,C70)</f>
-        <v>1200</v>
+        <v>2208</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -3868,7 +3869,7 @@
       </c>
       <c r="C72">
         <f>IF(C65&gt;C71,C65-C71,0)</f>
-        <v>3800</v>
+        <v>2792</v>
       </c>
       <c r="D72" t="s">
         <v>107</v>
@@ -3888,7 +3889,7 @@
       </c>
       <c r="C75" s="18">
         <f>$C$66*B75</f>
-        <v>1200</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -3908,9 +3909,9 @@
         <v>58</v>
       </c>
       <c r="B77" s="8"/>
-      <c r="C77">
+      <c r="C77" s="18">
         <f>MIN(C75,C76)</f>
-        <v>1200</v>
+        <v>2232</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -3919,7 +3920,7 @@
       </c>
       <c r="C78">
         <f>IF(C65&gt;C77,C65-C77,0)</f>
-        <v>3800</v>
+        <v>2768</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -3931,7 +3932,7 @@
       </c>
       <c r="C80" s="12">
         <f>$C$72*$B$80</f>
-        <v>570</v>
+        <v>418.8</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -3943,7 +3944,7 @@
       </c>
       <c r="C81" s="12">
         <f>$C$78*$B$81</f>
-        <v>191.9</v>
+        <v>139.78400000000002</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -3952,7 +3953,7 @@
       </c>
       <c r="C82" s="20">
         <f>SUM(C80:C81)</f>
-        <v>761.9</v>
+        <v>558.58400000000006</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -5629,7 +5630,7 @@
   </sheetPr>
   <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>